<commit_message>
Editing datasheet for privacy concerns
</commit_message>
<xml_diff>
--- a/Datasheet.xlsx
+++ b/Datasheet.xlsx
@@ -288,11 +288,11 @@
   </sheetPr>
   <dimension ref="A1:B1004"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A33" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2:B55"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D24" activeCellId="0" sqref="D24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="27.39"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="21.22"/>
@@ -311,7 +311,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="1" t="n">
-        <v>919897965441</v>
+        <v>9876543210</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -319,7 +319,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="1" t="n">
-        <v>9411020757</v>
+        <v>9876543211</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -327,7 +327,7 @@
         <v>4</v>
       </c>
       <c r="B4" s="1" t="n">
-        <v>9431346040</v>
+        <v>9876543212</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -335,7 +335,7 @@
         <v>5</v>
       </c>
       <c r="B5" s="1" t="n">
-        <v>919613448980</v>
+        <v>9876543213</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -343,7 +343,7 @@
         <v>6</v>
       </c>
       <c r="B6" s="1" t="n">
-        <v>9897965441</v>
+        <v>9876543214</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -351,7 +351,7 @@
         <v>7</v>
       </c>
       <c r="B7" s="1" t="n">
-        <v>918808653933</v>
+        <v>9876543215</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -359,7 +359,7 @@
         <v>8</v>
       </c>
       <c r="B8" s="1" t="n">
-        <v>918974859438</v>
+        <v>9876543216</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -367,7 +367,7 @@
         <v>9</v>
       </c>
       <c r="B9" s="1" t="n">
-        <v>9990490240</v>
+        <v>9876543217</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -375,7 +375,7 @@
         <v>10</v>
       </c>
       <c r="B10" s="1" t="n">
-        <v>8104195985</v>
+        <v>9876543218</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -383,7 +383,7 @@
         <v>11</v>
       </c>
       <c r="B11" s="1" t="n">
-        <v>9570208669</v>
+        <v>9876543219</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -391,7 +391,7 @@
         <v>12</v>
       </c>
       <c r="B12" s="1" t="n">
-        <v>919760606654</v>
+        <v>9876543220</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -399,7 +399,7 @@
         <v>13</v>
       </c>
       <c r="B13" s="1" t="n">
-        <v>918298151629</v>
+        <v>9876543221</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -407,7 +407,7 @@
         <v>14</v>
       </c>
       <c r="B14" s="1" t="n">
-        <v>919411020757</v>
+        <v>9876543222</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -415,7 +415,7 @@
         <v>15</v>
       </c>
       <c r="B15" s="1" t="n">
-        <v>9099932774</v>
+        <v>9876543223</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -423,7 +423,7 @@
         <v>16</v>
       </c>
       <c r="B16" s="1" t="n">
-        <v>917209167993</v>
+        <v>9876543224</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -431,7 +431,7 @@
         <v>17</v>
       </c>
       <c r="B17" s="1" t="n">
-        <v>9999007510</v>
+        <v>9876543225</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -439,7 +439,7 @@
         <v>18</v>
       </c>
       <c r="B18" s="1" t="n">
-        <v>9810895393</v>
+        <v>9876543226</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -447,7 +447,7 @@
         <v>19</v>
       </c>
       <c r="B19" s="1" t="n">
-        <v>9891681734</v>
+        <v>9876543227</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -455,7 +455,7 @@
         <v>20</v>
       </c>
       <c r="B20" s="1" t="n">
-        <v>8395274604</v>
+        <v>9876543228</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -463,7 +463,7 @@
         <v>21</v>
       </c>
       <c r="B21" s="1" t="n">
-        <v>9199414142</v>
+        <v>9876543229</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -471,7 +471,7 @@
         <v>22</v>
       </c>
       <c r="B22" s="1" t="n">
-        <v>911244985100</v>
+        <v>9876543230</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -479,7 +479,7 @@
         <v>23</v>
       </c>
       <c r="B23" s="1" t="n">
-        <v>919731878822</v>
+        <v>9876543231</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -487,7 +487,7 @@
         <v>24</v>
       </c>
       <c r="B24" s="1" t="n">
-        <v>8005592966</v>
+        <v>9876543232</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -495,7 +495,7 @@
         <v>25</v>
       </c>
       <c r="B25" s="1" t="n">
-        <v>919431346040</v>
+        <v>9876543233</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -503,7 +503,7 @@
         <v>26</v>
       </c>
       <c r="B26" s="1" t="n">
-        <v>9871962032</v>
+        <v>9876543234</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -511,7 +511,7 @@
         <v>27</v>
       </c>
       <c r="B27" s="1" t="n">
-        <v>8808653933</v>
+        <v>9876543235</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -519,7 +519,7 @@
         <v>28</v>
       </c>
       <c r="B28" s="1" t="n">
-        <v>8986461087</v>
+        <v>9876543236</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -527,7 +527,7 @@
         <v>28</v>
       </c>
       <c r="B29" s="1" t="n">
-        <v>9472868349</v>
+        <v>9876543237</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -535,7 +535,7 @@
         <v>29</v>
       </c>
       <c r="B30" s="1" t="n">
-        <v>8595225225</v>
+        <v>9876543238</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -543,7 +543,7 @@
         <v>30</v>
       </c>
       <c r="B31" s="1" t="n">
-        <v>9560945490</v>
+        <v>9876543239</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -551,7 +551,7 @@
         <v>31</v>
       </c>
       <c r="B32" s="1" t="n">
-        <v>919971350747</v>
+        <v>9876543240</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -559,7 +559,7 @@
         <v>32</v>
       </c>
       <c r="B33" s="1" t="n">
-        <v>918235433500</v>
+        <v>9876543241</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -567,7 +567,7 @@
         <v>33</v>
       </c>
       <c r="B34" s="1" t="n">
-        <v>918051157011</v>
+        <v>9876543242</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -575,7 +575,7 @@
         <v>34</v>
       </c>
       <c r="B35" s="1" t="n">
-        <v>8889973111</v>
+        <v>9876543243</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -583,7 +583,7 @@
         <v>35</v>
       </c>
       <c r="B36" s="1" t="n">
-        <v>919431853399</v>
+        <v>9876543244</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -591,7 +591,7 @@
         <v>36</v>
       </c>
       <c r="B37" s="1" t="n">
-        <v>9560063888</v>
+        <v>9876543245</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -599,7 +599,7 @@
         <v>37</v>
       </c>
       <c r="B38" s="1" t="n">
-        <v>919560945490</v>
+        <v>9876543246</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -607,7 +607,7 @@
         <v>38</v>
       </c>
       <c r="B39" s="1" t="n">
-        <v>919891725502</v>
+        <v>9876543247</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -615,7 +615,7 @@
         <v>39</v>
       </c>
       <c r="B40" s="1" t="n">
-        <v>911412785485</v>
+        <v>9876543248</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -623,7 +623,7 @@
         <v>40</v>
       </c>
       <c r="B41" s="1" t="n">
-        <v>919891150323</v>
+        <v>9876543249</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -631,7 +631,7 @@
         <v>41</v>
       </c>
       <c r="B42" s="1" t="n">
-        <v>6290247262</v>
+        <v>9876543250</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -639,7 +639,7 @@
         <v>42</v>
       </c>
       <c r="B43" s="1" t="n">
-        <v>9810672333</v>
+        <v>9876543251</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -647,7 +647,7 @@
         <v>43</v>
       </c>
       <c r="B44" s="1" t="n">
-        <v>9934005525</v>
+        <v>9876543252</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -655,7 +655,7 @@
         <v>44</v>
       </c>
       <c r="B45" s="1" t="n">
-        <v>8824740386</v>
+        <v>9876543253</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -663,7 +663,7 @@
         <v>45</v>
       </c>
       <c r="B46" s="1" t="n">
-        <v>911412785484</v>
+        <v>9876543254</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -671,7 +671,7 @@
         <v>46</v>
       </c>
       <c r="B47" s="1" t="n">
-        <v>919110972003</v>
+        <v>9876543255</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -679,7 +679,7 @@
         <v>47</v>
       </c>
       <c r="B48" s="1" t="n">
-        <v>8899973111</v>
+        <v>9876543256</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -687,7 +687,7 @@
         <v>48</v>
       </c>
       <c r="B49" s="1" t="n">
-        <v>9760606654</v>
+        <v>9876543257</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -695,7 +695,7 @@
         <v>49</v>
       </c>
       <c r="B50" s="1" t="n">
-        <v>9105683282212</v>
+        <v>9876543258</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -703,7 +703,7 @@
         <v>50</v>
       </c>
       <c r="B51" s="1" t="n">
-        <v>919740094239</v>
+        <v>9876543259</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -711,7 +711,7 @@
         <v>51</v>
       </c>
       <c r="B52" s="1" t="n">
-        <v>916204485041</v>
+        <v>9876543260</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -719,7 +719,7 @@
         <v>52</v>
       </c>
       <c r="B53" s="1" t="n">
-        <v>7974198697</v>
+        <v>9876543261</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -727,7 +727,7 @@
         <v>53</v>
       </c>
       <c r="B54" s="1" t="n">
-        <v>9971350747</v>
+        <v>9876543262</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -735,7 +735,7 @@
         <v>26</v>
       </c>
       <c r="B55" s="1" t="n">
-        <v>919871962032</v>
+        <v>9876543263</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>